<commit_message>
Improve eye opening mechanics.
Bugs reported: Cursor not rotating
</commit_message>
<xml_diff>
--- a/Bug Report.xlsx
+++ b/Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>BUG/BEHAVIOR</t>
   </si>
@@ -44,13 +44,25 @@
   </si>
   <si>
     <t>Eye closing animation not implemented, when alertness goes down it seems unnatural</t>
+  </si>
+  <si>
+    <t>Cursor not rotating</t>
+  </si>
+  <si>
+    <t>SOLVED?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,13 +70,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -113,16 +136,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,20 +452,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="71" customWidth="1"/>
-    <col min="2" max="3" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="41.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,11 +477,17 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -462,8 +497,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -473,8 +511,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -483,6 +524,23 @@
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve Alertness mechanism, update map, and various bug fixes
Alertness restructured to be simpler
Blocking wall behind the player is now invisible and made of Physics Volume
Add one more bot to test functionalities with 2 bots
</commit_message>
<xml_diff>
--- a/Bug Report.xlsx
+++ b/Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>BUG/BEHAVIOR</t>
   </si>
@@ -55,14 +55,23 @@
     <t>NO</t>
   </si>
   <si>
-    <t>REMARKS</t>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Bot/Player not totally dead after death.</t>
+  </si>
+  <si>
+    <t>PR0Pawn (presumably)</t>
+  </si>
+  <si>
+    <t>Maybe because Melkar override the deadanimation function?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,8 +85,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +102,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -136,20 +156,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +487,7 @@
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="41.44140625" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="6" max="6" width="43.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -483,9 +506,7 @@
       <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -497,8 +518,8 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
+      <c r="E2" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -511,8 +532,8 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -539,11 +560,29 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>